<commit_message>
combat is fully done now, all the way to reflex checks and skills
</commit_message>
<xml_diff>
--- a/assets/features.xlsx
+++ b/assets/features.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>Field</t>
   </si>
@@ -293,6 +293,90 @@
   </si>
   <si>
     <t>The screen should display player name and attributes</t>
+  </si>
+  <si>
+    <t>Implement Crissick</t>
+  </si>
+  <si>
+    <t>Implement Whirlwind</t>
+  </si>
+  <si>
+    <t>Implement The Void</t>
+  </si>
+  <si>
+    <t>Implement Observatory</t>
+  </si>
+  <si>
+    <t>Implement The Abyss</t>
+  </si>
+  <si>
+    <t>Implement Gadel Spyre</t>
+  </si>
+  <si>
+    <t>Implement Fulcrum</t>
+  </si>
+  <si>
+    <t>Implement Savanna</t>
+  </si>
+  <si>
+    <t>Implement Barrow</t>
+  </si>
+  <si>
+    <t>Implement Maelstrom</t>
+  </si>
+  <si>
+    <t>Implement Vault</t>
+  </si>
+  <si>
+    <t>Implement Nexus</t>
+  </si>
+  <si>
+    <t>Implement Darksun</t>
+  </si>
+  <si>
+    <t>Implement Badlands</t>
+  </si>
+  <si>
+    <t>Implement Lightway</t>
+  </si>
+  <si>
+    <t>Implement Eyes</t>
+  </si>
+  <si>
+    <t>Implement Darkstar</t>
+  </si>
+  <si>
+    <t>Implement Spacecom</t>
+  </si>
+  <si>
+    <t>Priorities:</t>
+  </si>
+  <si>
+    <t>Top current task: In Progress or High Priority</t>
+  </si>
+  <si>
+    <t>Next current tasks: Medium Priority</t>
+  </si>
+  <si>
+    <t>Top up next: Low Priority</t>
+  </si>
+  <si>
+    <t>Gronks can regenerate</t>
+  </si>
+  <si>
+    <t>Players are ejected when injured</t>
+  </si>
+  <si>
+    <t>Humans have Uncommon Valor</t>
+  </si>
+  <si>
+    <t>Sliths have Death Reek</t>
+  </si>
+  <si>
+    <t>Checks can have repulsor effects</t>
+  </si>
+  <si>
+    <t>The screen should alter the color of modified attributes</t>
   </si>
 </sst>
 </file>
@@ -405,7 +489,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -437,6 +521,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -448,7 +547,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -481,6 +580,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
@@ -792,7 +894,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +956,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -866,10 +968,10 @@
       <c r="D3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="12" t="s">
         <v>33</v>
       </c>
     </row>
@@ -886,10 +988,10 @@
       <c r="D4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -906,7 +1008,7 @@
       <c r="D5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="10" t="s">
         <v>48</v>
       </c>
       <c r="F5" t="s">
@@ -914,10 +1016,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="B6" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -926,15 +1031,21 @@
       <c r="E6" t="s">
         <v>50</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="A7" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E7" t="s">
@@ -942,13 +1053,16 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="A8" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E8" t="s">
@@ -956,13 +1070,16 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="A9" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E9" t="s">
@@ -970,13 +1087,16 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="A10" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E10" t="s">
@@ -984,13 +1104,16 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="A11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E11" t="s">
@@ -998,13 +1121,16 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="A12" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E12" t="s">
@@ -1012,13 +1138,16 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="A13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E13" t="s">
@@ -1026,13 +1155,16 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="A14" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>63</v>
       </c>
       <c r="E14" t="s">
@@ -1040,71 +1172,101 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="3" t="s">
+      <c r="A15" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="A16" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="3" t="s">
+      <c r="A17" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+      <c r="A18" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
+      <c r="A19" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
+      <c r="A20" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+      <c r="A21" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+      <c r="A22" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="3" t="s">
+      <c r="A23" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+      <c r="D24" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
+      <c r="D25" s="13" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+      <c r="D26" s="13" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1118,32 +1280,65 @@
         <v>86</v>
       </c>
     </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>117</v>
+      </c>
+    </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
skills panel done, player panel looking good, draft panel on its way
</commit_message>
<xml_diff>
--- a/assets/features.xlsx
+++ b/assets/features.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Version 1 (Clone)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t>Field</t>
   </si>
@@ -166,217 +166,292 @@
     <t>Equipment can modify attributes</t>
   </si>
   <si>
-    <t>Equipment can cause/resist shock effects</t>
-  </si>
-  <si>
-    <t>Equipment can cause/resist vortex effects</t>
+    <t>Equipment can cause/resist blob effects</t>
+  </si>
+  <si>
+    <t>Equipment can influence player appearance</t>
+  </si>
+  <si>
+    <t>Equipment can cause/resist injury</t>
+  </si>
+  <si>
+    <t>Equipment can cause backfire effects</t>
+  </si>
+  <si>
+    <t>Players can wear equipment</t>
+  </si>
+  <si>
+    <t>Equipment has a detection chance</t>
+  </si>
+  <si>
+    <t>Juggernaut prevents knockdown, setting AP to 0 instead</t>
+  </si>
+  <si>
+    <t>Checkmaster provides CH+10</t>
+  </si>
+  <si>
+    <t>Vicious adds to injury type</t>
+  </si>
+  <si>
+    <t>Resilient subtracts from injury type</t>
+  </si>
+  <si>
+    <t>Assists exist</t>
+  </si>
+  <si>
+    <t>Tactics negates assist bonuses when being checked</t>
+  </si>
+  <si>
+    <t>Brutal provides ST+10</t>
+  </si>
+  <si>
+    <t>Stalwart provides TG+10</t>
+  </si>
+  <si>
+    <t>Guard adds 50% to assist bonus</t>
+  </si>
+  <si>
+    <t>Doomstrike automatically injures target 25% of the time</t>
+  </si>
+  <si>
+    <t>Fist of Iron automatically stuns target 25% of the time</t>
+  </si>
+  <si>
+    <t>Quickening provides AP+10</t>
+  </si>
+  <si>
+    <t>Strip automatically steals ball from adjacent player 33%</t>
+  </si>
+  <si>
+    <t>Pickup is free with Scoop</t>
+  </si>
+  <si>
+    <t>Judo raises CH to that of attacker</t>
+  </si>
+  <si>
+    <t>Players reflex check twice with Combo</t>
+  </si>
+  <si>
+    <t>Juggling provides HD+10</t>
+  </si>
+  <si>
+    <t>Players can dodge attacks based on DA</t>
+  </si>
+  <si>
+    <t>Gymnastics provides DA+10</t>
+  </si>
+  <si>
+    <t>Gymnastics provides JP+10</t>
+  </si>
+  <si>
+    <t>Boxing provides RF+10</t>
+  </si>
+  <si>
+    <t>Include entries for all quirks and the following skills:</t>
+  </si>
+  <si>
+    <t>Terror</t>
+  </si>
+  <si>
+    <t>Sensei</t>
+  </si>
+  <si>
+    <t>Healer</t>
+  </si>
+  <si>
+    <t>Leader provides CH+5 for all friendlies within 5 tiles</t>
+  </si>
+  <si>
+    <t>Leader II</t>
+  </si>
+  <si>
+    <t>Karma reduces death to trivial injury once per season</t>
+  </si>
+  <si>
+    <t>Stoic</t>
+  </si>
+  <si>
+    <t>Awe prevents reflex checks 95% of the time unless Stoic</t>
+  </si>
+  <si>
+    <t>Sly cuts REF detection in half</t>
+  </si>
+  <si>
+    <t>Players can be ejected for equipment</t>
+  </si>
+  <si>
+    <t>Intuition doubles chance of successful ball bin</t>
+  </si>
+  <si>
+    <t>Implement Crissick</t>
+  </si>
+  <si>
+    <t>Implement Whirlwind</t>
+  </si>
+  <si>
+    <t>Implement The Void</t>
+  </si>
+  <si>
+    <t>Implement Observatory</t>
+  </si>
+  <si>
+    <t>Implement The Abyss</t>
+  </si>
+  <si>
+    <t>Implement Gadel Spyre</t>
+  </si>
+  <si>
+    <t>Implement Fulcrum</t>
+  </si>
+  <si>
+    <t>Implement Savanna</t>
+  </si>
+  <si>
+    <t>Implement Barrow</t>
+  </si>
+  <si>
+    <t>Implement Maelstrom</t>
+  </si>
+  <si>
+    <t>Implement Vault</t>
+  </si>
+  <si>
+    <t>Implement Nexus</t>
+  </si>
+  <si>
+    <t>Implement Darksun</t>
+  </si>
+  <si>
+    <t>Implement Badlands</t>
+  </si>
+  <si>
+    <t>Implement Lightway</t>
+  </si>
+  <si>
+    <t>Implement Eyes</t>
+  </si>
+  <si>
+    <t>Implement Darkstar</t>
+  </si>
+  <si>
+    <t>Implement Spacecom</t>
+  </si>
+  <si>
+    <t>Priorities:</t>
+  </si>
+  <si>
+    <t>Top current task: In Progress or High Priority</t>
+  </si>
+  <si>
+    <t>Next current tasks: Medium Priority</t>
+  </si>
+  <si>
+    <t>Top up next: Low Priority</t>
+  </si>
+  <si>
+    <t>Gronks can regenerate</t>
+  </si>
+  <si>
+    <t>Players are ejected when injured</t>
+  </si>
+  <si>
+    <t>Humans have Uncommon Valor</t>
+  </si>
+  <si>
+    <t>Sliths have Death Reek</t>
+  </si>
+  <si>
+    <t>Checks can have repulsor effects</t>
+  </si>
+  <si>
+    <t>The screen should alter the color of modified attributes</t>
+  </si>
+  <si>
+    <t>The screen should display player name and equipment</t>
+  </si>
+  <si>
+    <t>Kurgans have Bloodlust</t>
+  </si>
+  <si>
+    <t>Dragorans recover with only a 10AP penalty</t>
+  </si>
+  <si>
+    <t>Nynax boost the attributes of other Nynax</t>
+  </si>
+  <si>
+    <t>Races have a drafting cost</t>
+  </si>
+  <si>
+    <t>In-game actions provide XP</t>
+  </si>
+  <si>
+    <t>Players cost more money as their XP increases</t>
+  </si>
+  <si>
+    <t>XP can be used to purchase skills</t>
+  </si>
+  <si>
+    <t>Equipment has a purchase cost</t>
+  </si>
+  <si>
+    <t>Teams have a fixed budget of no more than 900K</t>
+  </si>
+  <si>
+    <t>Team stats, such as wins, are recorded</t>
+  </si>
+  <si>
+    <t>Individual stats, such as kills, are recorded</t>
+  </si>
+  <si>
+    <t>Teams can be saved and loaded to a file</t>
+  </si>
+  <si>
+    <t>Players may develop quirks after games</t>
+  </si>
+  <si>
+    <t>Teams can be managed from a window outside the game</t>
+  </si>
+  <si>
+    <t>Teams can be named</t>
+  </si>
+  <si>
+    <t>Teams can have coaches</t>
+  </si>
+  <si>
+    <t>Equipment can resist shock effects from tiles</t>
+  </si>
+  <si>
+    <t>Equipment can resist shock effects from surge gauntlets</t>
+  </si>
+  <si>
+    <t>Equipment can resist shock effects from surge armor</t>
+  </si>
+  <si>
+    <t>Equipment can cause shock effects</t>
+  </si>
+  <si>
+    <t>Equipment can cause vortex effects passively</t>
+  </si>
+  <si>
+    <t>Equipment can cause repulsor effects when attacking</t>
+  </si>
+  <si>
+    <t>Equipment can cause repulsor effects passively</t>
+  </si>
+  <si>
+    <t>Repulsor effects exist</t>
+  </si>
+  <si>
+    <t>Equipment can resist vortex effects</t>
+  </si>
+  <si>
+    <t>Teams for a new game can be imported from a file.</t>
+  </si>
+  <si>
+    <t>Events are ignored if the active player isn't the local computer</t>
   </si>
   <si>
     <t>Vortex effects exist</t>
-  </si>
-  <si>
-    <t>Equipment can cause/resist blob effects</t>
-  </si>
-  <si>
-    <t>Equipment can influence player appearance</t>
-  </si>
-  <si>
-    <t>Equipment can cause/resist injury</t>
-  </si>
-  <si>
-    <t>Equipment can cause backfire effects</t>
-  </si>
-  <si>
-    <t>Players can wear equipment</t>
-  </si>
-  <si>
-    <t>Equipment has a detection chance</t>
-  </si>
-  <si>
-    <t>Juggernaut prevents knockdown, setting AP to 0 instead</t>
-  </si>
-  <si>
-    <t>Checkmaster provides CH+10</t>
-  </si>
-  <si>
-    <t>Vicious adds to injury type</t>
-  </si>
-  <si>
-    <t>Resilient subtracts from injury type</t>
-  </si>
-  <si>
-    <t>Assists exist</t>
-  </si>
-  <si>
-    <t>Tactics negates assist bonuses when being checked</t>
-  </si>
-  <si>
-    <t>Brutal provides ST+10</t>
-  </si>
-  <si>
-    <t>Stalwart provides TG+10</t>
-  </si>
-  <si>
-    <t>Guard adds 50% to assist bonus</t>
-  </si>
-  <si>
-    <t>Doomstrike automatically injures target 25% of the time</t>
-  </si>
-  <si>
-    <t>Fist of Iron automatically stuns target 25% of the time</t>
-  </si>
-  <si>
-    <t>Quickening provides AP+10</t>
-  </si>
-  <si>
-    <t>Strip automatically steals ball from adjacent player 33%</t>
-  </si>
-  <si>
-    <t>Pickup is free with Scoop</t>
-  </si>
-  <si>
-    <t>Judo raises CH to that of attacker</t>
-  </si>
-  <si>
-    <t>Players reflex check twice with Combo</t>
-  </si>
-  <si>
-    <t>Juggling provides HD+10</t>
-  </si>
-  <si>
-    <t>Players can dodge attacks based on DA</t>
-  </si>
-  <si>
-    <t>Gymnastics provides DA+10</t>
-  </si>
-  <si>
-    <t>Gymnastics provides JP+10</t>
-  </si>
-  <si>
-    <t>Boxing provides RF+10</t>
-  </si>
-  <si>
-    <t>Include entries for all quirks and the following skills:</t>
-  </si>
-  <si>
-    <t>Terror</t>
-  </si>
-  <si>
-    <t>Sensei</t>
-  </si>
-  <si>
-    <t>Healer</t>
-  </si>
-  <si>
-    <t>Leader provides CH+5 for all friendlies within 5 tiles</t>
-  </si>
-  <si>
-    <t>Leader II</t>
-  </si>
-  <si>
-    <t>Karma reduces death to trivial injury once per season</t>
-  </si>
-  <si>
-    <t>Stoic</t>
-  </si>
-  <si>
-    <t>Awe prevents reflex checks 95% of the time unless Stoic</t>
-  </si>
-  <si>
-    <t>Sly cuts REF detection in half</t>
-  </si>
-  <si>
-    <t>Players can be ejected for equipment</t>
-  </si>
-  <si>
-    <t>Intuition doubles chance of successful ball bin</t>
-  </si>
-  <si>
-    <t>The screen should display player name and attributes</t>
-  </si>
-  <si>
-    <t>Implement Crissick</t>
-  </si>
-  <si>
-    <t>Implement Whirlwind</t>
-  </si>
-  <si>
-    <t>Implement The Void</t>
-  </si>
-  <si>
-    <t>Implement Observatory</t>
-  </si>
-  <si>
-    <t>Implement The Abyss</t>
-  </si>
-  <si>
-    <t>Implement Gadel Spyre</t>
-  </si>
-  <si>
-    <t>Implement Fulcrum</t>
-  </si>
-  <si>
-    <t>Implement Savanna</t>
-  </si>
-  <si>
-    <t>Implement Barrow</t>
-  </si>
-  <si>
-    <t>Implement Maelstrom</t>
-  </si>
-  <si>
-    <t>Implement Vault</t>
-  </si>
-  <si>
-    <t>Implement Nexus</t>
-  </si>
-  <si>
-    <t>Implement Darksun</t>
-  </si>
-  <si>
-    <t>Implement Badlands</t>
-  </si>
-  <si>
-    <t>Implement Lightway</t>
-  </si>
-  <si>
-    <t>Implement Eyes</t>
-  </si>
-  <si>
-    <t>Implement Darkstar</t>
-  </si>
-  <si>
-    <t>Implement Spacecom</t>
-  </si>
-  <si>
-    <t>Priorities:</t>
-  </si>
-  <si>
-    <t>Top current task: In Progress or High Priority</t>
-  </si>
-  <si>
-    <t>Next current tasks: Medium Priority</t>
-  </si>
-  <si>
-    <t>Top up next: Low Priority</t>
-  </si>
-  <si>
-    <t>Gronks can regenerate</t>
-  </si>
-  <si>
-    <t>Players are ejected when injured</t>
-  </si>
-  <si>
-    <t>Humans have Uncommon Valor</t>
-  </si>
-  <si>
-    <t>Sliths have Death Reek</t>
-  </si>
-  <si>
-    <t>Checks can have repulsor effects</t>
-  </si>
-  <si>
-    <t>The screen should alter the color of modified attributes</t>
   </si>
 </sst>
 </file>
@@ -547,7 +622,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -583,6 +658,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
@@ -894,12 +970,13 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="51.85546875" customWidth="1"/>
+    <col min="1" max="9" width="51.85546875" customWidth="1"/>
+    <col min="10" max="10" width="57.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="14" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -968,15 +1045,27 @@
       <c r="D3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>57</v>
+      <c r="E3" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>33</v>
       </c>
+      <c r="G3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -988,15 +1077,18 @@
       <c r="D4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>34</v>
       </c>
+      <c r="G4" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1008,16 +1100,19 @@
       <c r="D5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F5" t="s">
-        <v>92</v>
+      <c r="F5" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>93</v>
+      <c r="A6" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>42</v>
@@ -1029,15 +1124,18 @@
         <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>137</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="G6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>94</v>
+      <c r="A7" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>43</v>
@@ -1048,13 +1146,16 @@
       <c r="D7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
-        <v>51</v>
+      <c r="E7" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>95</v>
+      <c r="A8" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>44</v>
@@ -1066,12 +1167,15 @@
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>96</v>
+      <c r="A9" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>45</v>
@@ -1083,12 +1187,15 @@
         <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="G9" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>97</v>
+      <c r="A10" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>46</v>
@@ -1097,15 +1204,18 @@
         <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="G10" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>47</v>
@@ -1114,233 +1224,272 @@
         <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>52</v>
+        <v>95</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" t="s">
         <v>58</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" t="s">
-        <v>89</v>
+        <v>59</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="18" t="s">
+      <c r="D18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="D23" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D29" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D30" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>111</v>
-      </c>
       <c r="D32" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>119</v>
+        <v>108</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B34" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B35" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work begun on GUI overhaul.
</commit_message>
<xml_diff>
--- a/assets/features.xlsx
+++ b/assets/features.xlsx
@@ -622,7 +622,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -650,15 +650,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="7"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
@@ -969,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,7 +1030,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1048,10 +1045,10 @@
       <c r="E3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>121</v>
       </c>
       <c r="H3" t="s">
@@ -1080,10 +1077,10 @@
       <c r="E4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1106,7 +1103,7 @@
       <c r="F5" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="10" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1114,10 +1111,10 @@
       <c r="A6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1129,7 +1126,7 @@
       <c r="F6" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1137,19 +1134,19 @@
       <c r="A7" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1157,19 +1154,19 @@
       <c r="A8" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>40</v>
       </c>
       <c r="E8" t="s">
         <v>50</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="3" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1177,10 +1174,10 @@
       <c r="A9" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1189,7 +1186,7 @@
       <c r="E9" t="s">
         <v>51</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1197,10 +1194,10 @@
       <c r="A10" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1209,7 +1206,7 @@
       <c r="E10" t="s">
         <v>52</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1217,10 +1214,10 @@
       <c r="A11" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1229,18 +1226,18 @@
       <c r="E11" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B12" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1249,7 +1246,7 @@
       <c r="E12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="3" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1257,10 +1254,10 @@
       <c r="A13" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1274,13 +1271,13 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="16" t="s">
         <v>68</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1300,7 +1297,7 @@
       <c r="B15" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>69</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -1309,18 +1306,18 @@
       <c r="E15" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="14" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>72</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1331,13 +1328,13 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B17" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>88</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1348,7 +1345,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="3" t="s">
         <v>101</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1359,7 +1356,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="3" t="s">
         <v>102</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1370,7 +1367,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="3" t="s">
         <v>103</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -1381,41 +1378,41 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="12" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="12" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1445,10 +1442,10 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="13" t="s">
         <v>107</v>
       </c>
       <c r="D32" t="s">
@@ -1462,7 +1459,7 @@
       <c r="B33" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="14" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Team editor is pretty fleshed out now, and AI teams can draft players and equipment, as well as buying skills, arranging players, and otherwise managing the team.
</commit_message>
<xml_diff>
--- a/assets/features.xlsx
+++ b/assets/features.xlsx
@@ -654,8 +654,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
@@ -967,7 +967,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,7 +1277,7 @@
       <c r="B14" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>68</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1381,7 +1381,7 @@
       <c r="A21" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="16" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Team editor is almost entirely complete, with functional roster and settings screens.  Some quirks added.
</commit_message>
<xml_diff>
--- a/assets/features.xlsx
+++ b/assets/features.xlsx
@@ -966,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1051,7 @@
       <c r="G3" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>130</v>
       </c>
       <c r="I3" t="s">
@@ -1234,7 +1234,7 @@
       <c r="A12" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>120</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -1472,7 +1472,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B35" t="s">

</xml_diff>